<commit_message>
feat: add development assessment
</commit_message>
<xml_diff>
--- a/src/assessment_client/examples/stat_logic_example.xlsx
+++ b/src/assessment_client/examples/stat_logic_example.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="138">
   <si>
     <t>№</t>
   </si>
@@ -322,7 +322,7 @@
     <t>#27 задание Кейс 1</t>
   </si>
   <si>
-    <t>Ситуационные кейсы</t>
+    <t>Большие кейсы</t>
   </si>
   <si>
     <t xml:space="preserve"># Кейс 1
@@ -358,6 +358,9 @@
   </si>
   <si>
     <t>#28 задание Кейс 2</t>
+  </si>
+  <si>
+    <t>Мини кейсы</t>
   </si>
   <si>
     <t># Кейс 2
@@ -616,7 +619,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -655,6 +658,12 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Onest"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
@@ -798,7 +807,7 @@
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -1684,13 +1693,13 @@
         <v>73</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="D9" s="8" t="s">
         <v>23</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F9" s="9" t="s">
         <v>25</v>
@@ -1699,7 +1708,7 @@
         <v>47</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I9" s="10">
         <v>0.45</v>
@@ -1723,7 +1732,7 @@
         <v>25</v>
       </c>
       <c r="P9" s="13" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="Q9" s="14">
         <v>2</v>
@@ -1732,10 +1741,10 @@
         <f>Q9 * I9</f>
       </c>
       <c r="S9" s="8" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="T9" s="8" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="U9" s="16">
         <v>0</v>
@@ -1747,23 +1756,23 @@
         <v>3</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="D10" s="8" t="s">
         <v>23</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F10" s="9"/>
       <c r="G10" s="8" t="s">
         <v>54</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="I10" s="10">
         <v>0.45</v>
@@ -1787,7 +1796,7 @@
         <v>25</v>
       </c>
       <c r="P10" s="13" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="Q10" s="14">
         <v>3</v>
@@ -1796,10 +1805,10 @@
         <f>Q10 * I10</f>
       </c>
       <c r="S10" s="8" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="T10" s="8" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="U10" s="16">
         <v>0</v>
@@ -1811,16 +1820,16 @@
         <v>1</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D11" s="8" t="s">
         <v>23</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="F11" s="9" t="s">
         <v>25</v>
@@ -1853,7 +1862,7 @@
         <v>25</v>
       </c>
       <c r="P11" s="13" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="Q11" s="14">
         <v>0</v>
@@ -1862,7 +1871,7 @@
         <f>Q11 * I11</f>
       </c>
       <c r="S11" s="8" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="T11" s="8" t="s">
         <v>25</v>
@@ -1877,16 +1886,16 @@
         <v>1</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D12" s="8" t="s">
         <v>23</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="F12" s="9" t="s">
         <v>25</v>
@@ -1919,7 +1928,7 @@
         <v>25</v>
       </c>
       <c r="P12" s="13" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="Q12" s="14">
         <v>0</v>
@@ -1928,7 +1937,7 @@
         <f>Q12 * I12</f>
       </c>
       <c r="S12" s="8" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="T12" s="8" t="s">
         <v>25</v>
@@ -1943,16 +1952,16 @@
         <v>1</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D13" s="8" t="s">
         <v>23</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="F13" s="9" t="s">
         <v>25</v>
@@ -1985,7 +1994,7 @@
         <v>25</v>
       </c>
       <c r="P13" s="13" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="Q13" s="14">
         <v>0</v>
@@ -1994,7 +2003,7 @@
         <f>Q13 * I13</f>
       </c>
       <c r="S13" s="8" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="T13" s="8" t="s">
         <v>25</v>
@@ -2009,16 +2018,16 @@
         <v>1</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D14" s="8" t="s">
         <v>23</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="F14" s="9" t="s">
         <v>25</v>
@@ -2051,7 +2060,7 @@
         <v>25</v>
       </c>
       <c r="P14" s="13" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="Q14" s="14">
         <v>0</v>
@@ -2060,7 +2069,7 @@
         <f>Q14 * I14</f>
       </c>
       <c r="S14" s="8" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="T14" s="8" t="s">
         <v>25</v>
@@ -2075,16 +2084,16 @@
         <v>1</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D15" s="8" t="s">
         <v>23</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="F15" s="9" t="s">
         <v>25</v>
@@ -2117,7 +2126,7 @@
         <v>25</v>
       </c>
       <c r="P15" s="13" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="Q15" s="14">
         <v>0</v>
@@ -2126,7 +2135,7 @@
         <f>Q15 * I15</f>
       </c>
       <c r="S15" s="8" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="T15" s="8" t="s">
         <v>25</v>
@@ -2141,16 +2150,16 @@
         <v>1</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D16" s="8" t="s">
         <v>23</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="F16" s="9" t="s">
         <v>25</v>
@@ -2183,7 +2192,7 @@
         <v>25</v>
       </c>
       <c r="P16" s="13" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="Q16" s="14">
         <v>0</v>
@@ -2192,7 +2201,7 @@
         <f>Q16 * I16</f>
       </c>
       <c r="S16" s="8" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="T16" s="8" t="s">
         <v>25</v>
@@ -2207,19 +2216,19 @@
         <v>8</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D17" s="8" t="s">
         <v>23</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="F17" s="19" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="G17" s="8" t="s">
         <v>40</v>
@@ -2270,22 +2279,22 @@
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="17.25">
       <c r="A18" s="20" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D18" s="8" t="s">
         <v>23</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="F18" s="19" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="G18" s="8" t="s">
         <v>26</v>
@@ -2335,19 +2344,19 @@
         <v>15</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D19" s="8" t="s">
         <v>23</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="F19" s="19" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="G19" s="8" t="s">
         <v>33</v>
@@ -2397,19 +2406,19 @@
         <v>12</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D20" s="8" t="s">
         <v>23</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="F20" s="19" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="G20" s="8" t="s">
         <v>33</v>
@@ -2459,19 +2468,19 @@
         <v>9</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D21" s="8" t="s">
         <v>23</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="F21" s="19" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="G21" s="8" t="s">
         <v>47</v>
@@ -2521,19 +2530,19 @@
         <v>11</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D22" s="8" t="s">
         <v>23</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="F22" s="19" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="G22" s="8" t="s">
         <v>26</v>
@@ -2590,14 +2599,14 @@
         <v>23</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="F23" s="9"/>
       <c r="G23" s="8" t="s">
         <v>33</v>
       </c>
       <c r="H23" s="7" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="I23" s="10">
         <v>0.45</v>
@@ -2630,7 +2639,7 @@
         <f>Q23 * I23</f>
       </c>
       <c r="S23" s="8" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="T23" s="8" t="s">
         <v>72</v>
@@ -2645,19 +2654,19 @@
         <v>19</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D24" s="8" t="s">
         <v>23</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F24" s="19" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="G24" s="8" t="s">
         <v>26</v>
@@ -2711,19 +2720,19 @@
         <v>16</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D25" s="8" t="s">
         <v>23</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F25" s="19" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="G25" s="8" t="s">
         <v>33</v>
@@ -2773,19 +2782,19 @@
         <v>4</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D26" s="8" t="s">
         <v>23</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="F26" s="19" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="G26" s="8" t="s">
         <v>47</v>
@@ -2835,19 +2844,19 @@
         <v>1</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D27" s="8" t="s">
         <v>23</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="F27" s="19" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="G27" s="8" t="s">
         <v>26</v>
@@ -2897,19 +2906,19 @@
         <v>7</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D28" s="8" t="s">
         <v>23</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="F28" s="19" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="G28" s="8" t="s">
         <v>33</v>
@@ -2959,19 +2968,19 @@
         <v>2</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D29" s="8" t="s">
         <v>23</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="F29" s="19" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="G29" s="8" t="s">
         <v>33</v>
@@ -3021,19 +3030,19 @@
         <v>18</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D30" s="8" t="s">
         <v>23</v>
       </c>
       <c r="E30" s="8" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F30" s="19" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="G30" s="8" t="s">
         <v>61</v>
@@ -3083,19 +3092,19 @@
         <v>10</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D31" s="8" t="s">
         <v>23</v>
       </c>
       <c r="E31" s="8" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="F31" s="19" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="G31" s="8" t="s">
         <v>54</v>
@@ -3145,19 +3154,19 @@
         <v>5</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D32" s="8" t="s">
         <v>23</v>
       </c>
       <c r="E32" s="8" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="F32" s="19" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="G32" s="8" t="s">
         <v>61</v>
@@ -3207,19 +3216,19 @@
         <v>20</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D33" s="8" t="s">
         <v>23</v>
       </c>
       <c r="E33" s="8" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="F33" s="19" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="G33" s="8" t="s">
         <v>54</v>
@@ -3269,19 +3278,19 @@
         <v>13</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D34" s="8" t="s">
         <v>23</v>
       </c>
       <c r="E34" s="8" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="F34" s="19" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="G34" s="8" t="s">
         <v>47</v>
@@ -3331,19 +3340,19 @@
         <v>14</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D35" s="8" t="s">
         <v>23</v>
       </c>
       <c r="E35" s="8" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F35" s="19" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="G35" s="8" t="s">
         <v>26</v>
@@ -3393,19 +3402,19 @@
         <v>3</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D36" s="8" t="s">
         <v>23</v>
       </c>
       <c r="E36" s="8" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="F36" s="19" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="G36" s="8" t="s">
         <v>40</v>
@@ -3455,19 +3464,19 @@
         <v>17</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D37" s="8" t="s">
         <v>23</v>
       </c>
       <c r="E37" s="8" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="F37" s="19" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="G37" s="8" t="s">
         <v>40</v>

</xml_diff>